<commit_message>
rankings no funcional + arreglos toolbar
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 5ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 5ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7E62DC-67E8-4986-B7E1-C2FE7F655C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED655440-6193-497D-A8BD-CE71F096E96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -653,9 +653,6 @@
     <t>cartas de eleccion</t>
   </si>
   <si>
-    <t>interfaz de ajustes</t>
-  </si>
-  <si>
     <t>Termina bingo de 90 bolas</t>
   </si>
   <si>
@@ -663,6 +660,9 @@
   </si>
   <si>
     <t>Carteles juegos dados + frontal</t>
+  </si>
+  <si>
+    <t>interfaz de ajustes (continuacion)</t>
   </si>
 </sst>
 </file>
@@ -2205,8 +2205,8 @@
   </sheetPr>
   <dimension ref="A2:P154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K149" sqref="K149"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C151" sqref="C151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2260,7 +2260,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>408.53000000000003</v>
+        <v>410.03000000000003</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
@@ -2384,7 +2384,7 @@
       </c>
       <c r="K9" s="66">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74+J131+J146</f>
-        <v>90.93</v>
+        <v>92.43</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -5027,7 +5027,7 @@
       </c>
       <c r="J146">
         <f>F148+F149+F150+F151</f>
-        <v>0.67</v>
+        <v>2.17</v>
       </c>
       <c r="K146">
         <f>E148+E149+E150+E151</f>
@@ -5060,7 +5060,10 @@
         <v>9</v>
       </c>
       <c r="E148" s="13"/>
-      <c r="F148" s="13"/>
+      <c r="F148" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="G148" s="11"/>
       <c r="I148" s="5" t="s">
         <v>12</v>
       </c>
@@ -5116,7 +5119,7 @@
         <v>13</v>
       </c>
       <c r="C151" s="13" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D151" s="15">
         <v>39</v>
@@ -5130,7 +5133,7 @@
         <v>9</v>
       </c>
       <c r="C152" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D152" s="13">
         <v>24</v>
@@ -5148,7 +5151,7 @@
         <v>9</v>
       </c>
       <c r="C153" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D153" s="13">
         <v>35</v>
@@ -5164,7 +5167,7 @@
         <v>9</v>
       </c>
       <c r="C154" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D154" s="13" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Excel y cambios craps
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 5ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 5ª Version.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7nume\OneDrive\Documentos\CEU\3- Tercero\Software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683F670B-8AE1-45A5-8E6D-2E5642F4B8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20156B2D-9DFE-4BF2-9139-1B1283F1CA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="200">
   <si>
     <t>Nombre</t>
   </si>
@@ -663,6 +663,9 @@
   </si>
   <si>
     <t>interfaz de ajustes (continuacion)</t>
+  </si>
+  <si>
+    <t>Lógica 1 jugador Póker Texas</t>
   </si>
 </sst>
 </file>
@@ -1116,10 +1119,19 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1128,25 +1140,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1176,14 +1170,23 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2203,10 +2206,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:P154"/>
+  <dimension ref="A2:P156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J155" activeCellId="1" sqref="F150 J155"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E160" sqref="E160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2256,42 +2259,42 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E996)</f>
-        <v>327.2</v>
+        <v>328.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>411.53000000000003</v>
+        <v>413.03000000000003</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="72">
+      <c r="K3" s="69">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130</f>
         <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="72"/>
+      <c r="K4" s="69"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="61"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="72"/>
+      <c r="K5" s="69"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2311,7 +2314,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="73" t="s">
+      <c r="J6" s="70" t="s">
         <v>12</v>
       </c>
       <c r="K6" s="66">
@@ -2337,7 +2340,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="74"/>
+      <c r="J7" s="71"/>
       <c r="K7" s="66"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -2358,7 +2361,7 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="75"/>
+      <c r="J8" s="72"/>
       <c r="K8" s="66"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -2379,7 +2382,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="76" t="s">
+      <c r="J9" s="73" t="s">
         <v>13</v>
       </c>
       <c r="K9" s="66">
@@ -2404,7 +2407,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="77"/>
+      <c r="J10" s="74"/>
       <c r="K10" s="66"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2422,7 +2425,7 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="78"/>
+      <c r="J11" s="75"/>
       <c r="K11" s="66"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -2442,7 +2445,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="63" t="s">
+      <c r="J12" s="76" t="s">
         <v>14</v>
       </c>
       <c r="K12" s="66">
@@ -2465,7 +2468,7 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="64"/>
+      <c r="J13" s="77"/>
       <c r="K13" s="66"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2483,7 +2486,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="65"/>
+      <c r="J14" s="78"/>
       <c r="K14" s="66"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2501,7 +2504,7 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="67" t="s">
+      <c r="J15" s="79" t="s">
         <v>15</v>
       </c>
       <c r="K15" s="66">
@@ -2524,7 +2527,7 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="68"/>
+      <c r="J16" s="80"/>
       <c r="K16" s="66"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2542,7 +2545,7 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="69"/>
+      <c r="J17" s="81"/>
       <c r="K17" s="66"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2562,7 +2565,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="70" t="s">
+      <c r="J18" s="67" t="s">
         <v>16</v>
       </c>
       <c r="K18" s="66">
@@ -2588,7 +2591,7 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="71"/>
+      <c r="J19" s="68"/>
       <c r="K19" s="66"/>
     </row>
     <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
@@ -2608,7 +2611,7 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="71"/>
+      <c r="J20" s="68"/>
       <c r="K20" s="66"/>
     </row>
     <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
@@ -2646,11 +2649,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="79" t="s">
+      <c r="J22" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="79"/>
-      <c r="L22" s="79"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
     </row>
     <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -2974,22 +2977,22 @@
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B41" s="59" t="s">
+      <c r="B41" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="60"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="61"/>
     </row>
     <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="61"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="62"/>
+      <c r="B42" s="64"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="65"/>
+      <c r="G42" s="65"/>
     </row>
     <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
@@ -3661,14 +3664,14 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="59" t="s">
+      <c r="B72" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="60"/>
-      <c r="D72" s="60"/>
-      <c r="E72" s="60"/>
-      <c r="F72" s="60"/>
-      <c r="G72" s="60"/>
+      <c r="C72" s="61"/>
+      <c r="D72" s="61"/>
+      <c r="E72" s="61"/>
+      <c r="F72" s="61"/>
+      <c r="G72" s="61"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3680,12 +3683,12 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="61"/>
-      <c r="C73" s="62"/>
-      <c r="D73" s="62"/>
-      <c r="E73" s="62"/>
-      <c r="F73" s="62"/>
-      <c r="G73" s="62"/>
+      <c r="B73" s="64"/>
+      <c r="C73" s="65"/>
+      <c r="D73" s="65"/>
+      <c r="E73" s="65"/>
+      <c r="F73" s="65"/>
+      <c r="G73" s="65"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -4645,22 +4648,22 @@
       <c r="G126" s="50"/>
     </row>
     <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="59" t="s">
+      <c r="B127" s="60" t="s">
         <v>176</v>
       </c>
-      <c r="C127" s="60"/>
-      <c r="D127" s="60"/>
-      <c r="E127" s="60"/>
-      <c r="F127" s="60"/>
-      <c r="G127" s="60"/>
+      <c r="C127" s="61"/>
+      <c r="D127" s="61"/>
+      <c r="E127" s="61"/>
+      <c r="F127" s="61"/>
+      <c r="G127" s="61"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="80"/>
-      <c r="C128" s="81"/>
-      <c r="D128" s="81"/>
-      <c r="E128" s="81"/>
-      <c r="F128" s="81"/>
-      <c r="G128" s="81"/>
+      <c r="B128" s="62"/>
+      <c r="C128" s="63"/>
+      <c r="D128" s="63"/>
+      <c r="E128" s="63"/>
+      <c r="F128" s="63"/>
+      <c r="G128" s="63"/>
     </row>
     <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="51" t="s">
@@ -4946,22 +4949,22 @@
       <c r="G141" s="7"/>
     </row>
     <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="59" t="s">
+      <c r="B142" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="C142" s="60"/>
-      <c r="D142" s="60"/>
-      <c r="E142" s="60"/>
-      <c r="F142" s="60"/>
-      <c r="G142" s="60"/>
+      <c r="C142" s="61"/>
+      <c r="D142" s="61"/>
+      <c r="E142" s="61"/>
+      <c r="F142" s="61"/>
+      <c r="G142" s="61"/>
     </row>
     <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="80"/>
-      <c r="C143" s="81"/>
-      <c r="D143" s="81"/>
-      <c r="E143" s="81"/>
-      <c r="F143" s="81"/>
-      <c r="G143" s="81"/>
+      <c r="B143" s="62"/>
+      <c r="C143" s="63"/>
+      <c r="D143" s="63"/>
+      <c r="E143" s="63"/>
+      <c r="F143" s="63"/>
+      <c r="G143" s="63"/>
     </row>
     <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="55" t="s">
@@ -5178,13 +5181,43 @@
       <c r="F154" s="13"/>
       <c r="G154" s="26"/>
     </row>
+    <row r="155" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B155" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C155" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="D155" s="13"/>
+      <c r="E155" s="13">
+        <v>1</v>
+      </c>
+      <c r="F155" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="G155" s="11"/>
+    </row>
+    <row r="156" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C156" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D156" s="13">
+        <v>15</v>
+      </c>
+      <c r="E156" s="13"/>
+      <c r="F156" s="13"/>
+      <c r="G156" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="B142:G143"/>
-    <mergeCell ref="B127:G128"/>
-    <mergeCell ref="B72:G73"/>
-    <mergeCell ref="B41:G42"/>
+    <mergeCell ref="B4:G5"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="K15:K17"/>
     <mergeCell ref="K18:K20"/>
     <mergeCell ref="J18:J20"/>
     <mergeCell ref="K3:K5"/>
@@ -5192,11 +5225,11 @@
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
-    <mergeCell ref="B4:G5"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="B142:G143"/>
+    <mergeCell ref="B127:G128"/>
+    <mergeCell ref="B72:G73"/>
+    <mergeCell ref="B41:G42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5212,7 +5245,7 @@
   </sheetPr>
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
@@ -6182,6 +6215,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6390,38 +6440,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6444,9 +6466,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Soporte tecnico funcional y excel
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 5ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 5ª Version.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7nume\OneDrive\Documentos\CEU\3- Tercero\Software\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20156B2D-9DFE-4BF2-9139-1B1283F1CA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A548E8-0254-4D15-83BE-7C0937CCF18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -1119,19 +1119,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1140,7 +1131,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1170,23 +1179,14 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2209,7 +2209,7 @@
   <dimension ref="A2:P156"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A132" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E160" sqref="E160"/>
+      <selection activeCell="J149" sqref="J149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2259,42 +2259,42 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E996)</f>
-        <v>328.2</v>
+        <v>330.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>413.03000000000003</v>
+        <v>420.03000000000003</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="69">
+      <c r="K3" s="72">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130</f>
         <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="69"/>
+      <c r="K4" s="72"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="64"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="69"/>
+      <c r="K5" s="72"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2314,7 +2314,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="70" t="s">
+      <c r="J6" s="73" t="s">
         <v>12</v>
       </c>
       <c r="K6" s="66">
@@ -2340,7 +2340,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="71"/>
+      <c r="J7" s="74"/>
       <c r="K7" s="66"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -2361,7 +2361,7 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="72"/>
+      <c r="J8" s="75"/>
       <c r="K8" s="66"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -2382,7 +2382,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="73" t="s">
+      <c r="J9" s="76" t="s">
         <v>13</v>
       </c>
       <c r="K9" s="66">
@@ -2407,7 +2407,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="74"/>
+      <c r="J10" s="77"/>
       <c r="K10" s="66"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2425,7 +2425,7 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="75"/>
+      <c r="J11" s="78"/>
       <c r="K11" s="66"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -2445,7 +2445,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="76" t="s">
+      <c r="J12" s="63" t="s">
         <v>14</v>
       </c>
       <c r="K12" s="66">
@@ -2468,7 +2468,7 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="77"/>
+      <c r="J13" s="64"/>
       <c r="K13" s="66"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2486,7 +2486,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="78"/>
+      <c r="J14" s="65"/>
       <c r="K14" s="66"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2504,7 +2504,7 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="79" t="s">
+      <c r="J15" s="67" t="s">
         <v>15</v>
       </c>
       <c r="K15" s="66">
@@ -2527,7 +2527,7 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="80"/>
+      <c r="J16" s="68"/>
       <c r="K16" s="66"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2545,7 +2545,7 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="81"/>
+      <c r="J17" s="69"/>
       <c r="K17" s="66"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2565,7 +2565,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="67" t="s">
+      <c r="J18" s="70" t="s">
         <v>16</v>
       </c>
       <c r="K18" s="66">
@@ -2591,7 +2591,7 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="68"/>
+      <c r="J19" s="71"/>
       <c r="K19" s="66"/>
     </row>
     <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
@@ -2611,7 +2611,7 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="68"/>
+      <c r="J20" s="71"/>
       <c r="K20" s="66"/>
     </row>
     <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
@@ -2649,11 +2649,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="59" t="s">
+      <c r="J22" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="59"/>
-      <c r="L22" s="59"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="79"/>
     </row>
     <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -2977,22 +2977,22 @@
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B41" s="60" t="s">
+      <c r="B41" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
     </row>
     <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="64"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
     </row>
     <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
@@ -3664,14 +3664,14 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="60" t="s">
+      <c r="B72" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="61"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="61"/>
-      <c r="G72" s="61"/>
+      <c r="C72" s="60"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="60"/>
+      <c r="F72" s="60"/>
+      <c r="G72" s="60"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3683,12 +3683,12 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="64"/>
-      <c r="C73" s="65"/>
-      <c r="D73" s="65"/>
-      <c r="E73" s="65"/>
-      <c r="F73" s="65"/>
-      <c r="G73" s="65"/>
+      <c r="B73" s="61"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="62"/>
+      <c r="E73" s="62"/>
+      <c r="F73" s="62"/>
+      <c r="G73" s="62"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -4648,22 +4648,22 @@
       <c r="G126" s="50"/>
     </row>
     <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="60" t="s">
+      <c r="B127" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="C127" s="61"/>
-      <c r="D127" s="61"/>
-      <c r="E127" s="61"/>
-      <c r="F127" s="61"/>
-      <c r="G127" s="61"/>
+      <c r="C127" s="60"/>
+      <c r="D127" s="60"/>
+      <c r="E127" s="60"/>
+      <c r="F127" s="60"/>
+      <c r="G127" s="60"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="62"/>
-      <c r="C128" s="63"/>
-      <c r="D128" s="63"/>
-      <c r="E128" s="63"/>
-      <c r="F128" s="63"/>
-      <c r="G128" s="63"/>
+      <c r="B128" s="80"/>
+      <c r="C128" s="81"/>
+      <c r="D128" s="81"/>
+      <c r="E128" s="81"/>
+      <c r="F128" s="81"/>
+      <c r="G128" s="81"/>
     </row>
     <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="51" t="s">
@@ -4949,22 +4949,22 @@
       <c r="G141" s="7"/>
     </row>
     <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="60" t="s">
+      <c r="B142" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="C142" s="61"/>
-      <c r="D142" s="61"/>
-      <c r="E142" s="61"/>
-      <c r="F142" s="61"/>
-      <c r="G142" s="61"/>
+      <c r="C142" s="60"/>
+      <c r="D142" s="60"/>
+      <c r="E142" s="60"/>
+      <c r="F142" s="60"/>
+      <c r="G142" s="60"/>
     </row>
     <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="62"/>
-      <c r="C143" s="63"/>
-      <c r="D143" s="63"/>
-      <c r="E143" s="63"/>
-      <c r="F143" s="63"/>
-      <c r="G143" s="63"/>
+      <c r="B143" s="80"/>
+      <c r="C143" s="81"/>
+      <c r="D143" s="81"/>
+      <c r="E143" s="81"/>
+      <c r="F143" s="81"/>
+      <c r="G143" s="81"/>
     </row>
     <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="55" t="s">
@@ -4999,8 +4999,12 @@
         <v>190</v>
       </c>
       <c r="D145" s="13"/>
-      <c r="E145" s="13"/>
-      <c r="F145" s="13"/>
+      <c r="E145" s="13">
+        <v>2</v>
+      </c>
+      <c r="F145" s="13">
+        <v>7</v>
+      </c>
       <c r="G145" s="13"/>
       <c r="I145" s="57" t="s">
         <v>9</v>
@@ -5071,12 +5075,12 @@
         <v>12</v>
       </c>
       <c r="J148">
-        <f>F144</f>
+        <f>F144+F145+F147</f>
+        <v>10</v>
+      </c>
+      <c r="K148">
+        <f>E144+E145+E147</f>
         <v>3</v>
-      </c>
-      <c r="K148">
-        <f>E144</f>
-        <v>1</v>
       </c>
     </row>
     <row r="149" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5213,11 +5217,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B4:G5"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="B142:G143"/>
+    <mergeCell ref="B127:G128"/>
+    <mergeCell ref="B72:G73"/>
+    <mergeCell ref="B41:G42"/>
     <mergeCell ref="K18:K20"/>
     <mergeCell ref="J18:J20"/>
     <mergeCell ref="K3:K5"/>
@@ -5225,11 +5229,11 @@
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="B142:G143"/>
-    <mergeCell ref="B127:G128"/>
-    <mergeCell ref="B72:G73"/>
-    <mergeCell ref="B41:G42"/>
+    <mergeCell ref="B4:G5"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="K15:K17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6215,23 +6219,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6440,10 +6427,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6466,20 +6481,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
algo mas de ajustes de perfil
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 5ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 5ª Version.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7nume\OneDrive\Documentos\CEU\3- Tercero\Software\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20156B2D-9DFE-4BF2-9139-1B1283F1CA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C32B3C-DCD5-4B78-BCFA-9A0DBA997EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -1119,19 +1119,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1140,7 +1131,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1170,23 +1179,14 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2208,8 +2208,8 @@
   </sheetPr>
   <dimension ref="A2:P156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E160" sqref="E160"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F150" sqref="F150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2263,38 +2263,38 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>413.03000000000003</v>
+        <v>414.53000000000003</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="69">
+      <c r="K3" s="72">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130</f>
         <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="69"/>
+      <c r="K4" s="72"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="64"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="69"/>
+      <c r="K5" s="72"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2314,7 +2314,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="70" t="s">
+      <c r="J6" s="73" t="s">
         <v>12</v>
       </c>
       <c r="K6" s="66">
@@ -2340,7 +2340,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="71"/>
+      <c r="J7" s="74"/>
       <c r="K7" s="66"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -2361,7 +2361,7 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="72"/>
+      <c r="J8" s="75"/>
       <c r="K8" s="66"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -2382,12 +2382,12 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="73" t="s">
+      <c r="J9" s="76" t="s">
         <v>13</v>
       </c>
       <c r="K9" s="66">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+J74+J131+J146</f>
-        <v>93.93</v>
+        <v>95.43</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -2407,7 +2407,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="74"/>
+      <c r="J10" s="77"/>
       <c r="K10" s="66"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2425,7 +2425,7 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="75"/>
+      <c r="J11" s="78"/>
       <c r="K11" s="66"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -2445,7 +2445,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="76" t="s">
+      <c r="J12" s="63" t="s">
         <v>14</v>
       </c>
       <c r="K12" s="66">
@@ -2468,7 +2468,7 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="77"/>
+      <c r="J13" s="64"/>
       <c r="K13" s="66"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2486,7 +2486,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="78"/>
+      <c r="J14" s="65"/>
       <c r="K14" s="66"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2504,7 +2504,7 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="79" t="s">
+      <c r="J15" s="67" t="s">
         <v>15</v>
       </c>
       <c r="K15" s="66">
@@ -2527,7 +2527,7 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="80"/>
+      <c r="J16" s="68"/>
       <c r="K16" s="66"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2545,7 +2545,7 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="81"/>
+      <c r="J17" s="69"/>
       <c r="K17" s="66"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2565,7 +2565,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="67" t="s">
+      <c r="J18" s="70" t="s">
         <v>16</v>
       </c>
       <c r="K18" s="66">
@@ -2591,7 +2591,7 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="68"/>
+      <c r="J19" s="71"/>
       <c r="K19" s="66"/>
     </row>
     <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
@@ -2611,7 +2611,7 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="68"/>
+      <c r="J20" s="71"/>
       <c r="K20" s="66"/>
     </row>
     <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
@@ -2649,11 +2649,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="59" t="s">
+      <c r="J22" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="59"/>
-      <c r="L22" s="59"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="79"/>
     </row>
     <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -2977,22 +2977,22 @@
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B41" s="60" t="s">
+      <c r="B41" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
     </row>
     <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="64"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
     </row>
     <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
@@ -3664,14 +3664,14 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="60" t="s">
+      <c r="B72" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="61"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="61"/>
-      <c r="G72" s="61"/>
+      <c r="C72" s="60"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="60"/>
+      <c r="F72" s="60"/>
+      <c r="G72" s="60"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3683,12 +3683,12 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="64"/>
-      <c r="C73" s="65"/>
-      <c r="D73" s="65"/>
-      <c r="E73" s="65"/>
-      <c r="F73" s="65"/>
-      <c r="G73" s="65"/>
+      <c r="B73" s="61"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="62"/>
+      <c r="E73" s="62"/>
+      <c r="F73" s="62"/>
+      <c r="G73" s="62"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -4648,22 +4648,22 @@
       <c r="G126" s="50"/>
     </row>
     <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="60" t="s">
+      <c r="B127" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="C127" s="61"/>
-      <c r="D127" s="61"/>
-      <c r="E127" s="61"/>
-      <c r="F127" s="61"/>
-      <c r="G127" s="61"/>
+      <c r="C127" s="60"/>
+      <c r="D127" s="60"/>
+      <c r="E127" s="60"/>
+      <c r="F127" s="60"/>
+      <c r="G127" s="60"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="62"/>
-      <c r="C128" s="63"/>
-      <c r="D128" s="63"/>
-      <c r="E128" s="63"/>
-      <c r="F128" s="63"/>
-      <c r="G128" s="63"/>
+      <c r="B128" s="80"/>
+      <c r="C128" s="81"/>
+      <c r="D128" s="81"/>
+      <c r="E128" s="81"/>
+      <c r="F128" s="81"/>
+      <c r="G128" s="81"/>
     </row>
     <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="51" t="s">
@@ -4949,22 +4949,22 @@
       <c r="G141" s="7"/>
     </row>
     <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="60" t="s">
+      <c r="B142" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="C142" s="61"/>
-      <c r="D142" s="61"/>
-      <c r="E142" s="61"/>
-      <c r="F142" s="61"/>
-      <c r="G142" s="61"/>
+      <c r="C142" s="60"/>
+      <c r="D142" s="60"/>
+      <c r="E142" s="60"/>
+      <c r="F142" s="60"/>
+      <c r="G142" s="60"/>
     </row>
     <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="62"/>
-      <c r="C143" s="63"/>
-      <c r="D143" s="63"/>
-      <c r="E143" s="63"/>
-      <c r="F143" s="63"/>
-      <c r="G143" s="63"/>
+      <c r="B143" s="80"/>
+      <c r="C143" s="81"/>
+      <c r="D143" s="81"/>
+      <c r="E143" s="81"/>
+      <c r="F143" s="81"/>
+      <c r="G143" s="81"/>
     </row>
     <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="55" t="s">
@@ -5030,7 +5030,7 @@
       </c>
       <c r="J146">
         <f>F148+F149+F150+F151</f>
-        <v>3.67</v>
+        <v>5.17</v>
       </c>
       <c r="K146">
         <f>E148+E149+E150+E151</f>
@@ -5064,7 +5064,7 @@
       </c>
       <c r="E148" s="13"/>
       <c r="F148" s="13">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="G148" s="11"/>
       <c r="I148" s="5" t="s">
@@ -5093,7 +5093,7 @@
         <v>3</v>
       </c>
       <c r="F149" s="13">
-        <v>1.17</v>
+        <v>1.67</v>
       </c>
       <c r="G149" s="11"/>
       <c r="I149" s="8" t="s">
@@ -5213,11 +5213,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B4:G5"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="B142:G143"/>
+    <mergeCell ref="B127:G128"/>
+    <mergeCell ref="B72:G73"/>
+    <mergeCell ref="B41:G42"/>
     <mergeCell ref="K18:K20"/>
     <mergeCell ref="J18:J20"/>
     <mergeCell ref="K3:K5"/>
@@ -5225,11 +5225,11 @@
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="B142:G143"/>
-    <mergeCell ref="B127:G128"/>
-    <mergeCell ref="B72:G73"/>
-    <mergeCell ref="B41:G42"/>
+    <mergeCell ref="B4:G5"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="K15:K17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6215,23 +6215,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6440,10 +6423,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6466,20 +6477,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Excel PORFAVOR NO ME BORREN OTRA VEZ EL EXCEL y metida desafios y recompensas en plantilla
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 5ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 5ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C32B3C-DCD5-4B78-BCFA-9A0DBA997EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF9CFFE-BC0E-4F4C-AD5D-0571A92D43A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -1119,10 +1119,19 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1131,25 +1140,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1179,14 +1170,23 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2208,8 +2208,8 @@
   </sheetPr>
   <dimension ref="A2:P156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F150" sqref="F150"/>
+    <sheetView topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B142" sqref="B142:G143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2259,42 +2259,42 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E996)</f>
-        <v>328.2</v>
+        <v>330.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>414.53000000000003</v>
+        <v>421.53000000000003</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="72">
+      <c r="K3" s="69">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130</f>
         <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="72"/>
+      <c r="K4" s="69"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="61"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="72"/>
+      <c r="K5" s="69"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2314,7 +2314,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="73" t="s">
+      <c r="J6" s="70" t="s">
         <v>12</v>
       </c>
       <c r="K6" s="66">
@@ -2340,7 +2340,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="74"/>
+      <c r="J7" s="71"/>
       <c r="K7" s="66"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -2361,7 +2361,7 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="75"/>
+      <c r="J8" s="72"/>
       <c r="K8" s="66"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -2382,7 +2382,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="76" t="s">
+      <c r="J9" s="73" t="s">
         <v>13</v>
       </c>
       <c r="K9" s="66">
@@ -2407,7 +2407,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="77"/>
+      <c r="J10" s="74"/>
       <c r="K10" s="66"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2425,7 +2425,7 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="78"/>
+      <c r="J11" s="75"/>
       <c r="K11" s="66"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -2445,7 +2445,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="63" t="s">
+      <c r="J12" s="76" t="s">
         <v>14</v>
       </c>
       <c r="K12" s="66">
@@ -2468,7 +2468,7 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="64"/>
+      <c r="J13" s="77"/>
       <c r="K13" s="66"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2486,7 +2486,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="65"/>
+      <c r="J14" s="78"/>
       <c r="K14" s="66"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2504,7 +2504,7 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="67" t="s">
+      <c r="J15" s="79" t="s">
         <v>15</v>
       </c>
       <c r="K15" s="66">
@@ -2527,7 +2527,7 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="68"/>
+      <c r="J16" s="80"/>
       <c r="K16" s="66"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2545,7 +2545,7 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="69"/>
+      <c r="J17" s="81"/>
       <c r="K17" s="66"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2565,7 +2565,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="70" t="s">
+      <c r="J18" s="67" t="s">
         <v>16</v>
       </c>
       <c r="K18" s="66">
@@ -2591,7 +2591,7 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="71"/>
+      <c r="J19" s="68"/>
       <c r="K19" s="66"/>
     </row>
     <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
@@ -2611,7 +2611,7 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="71"/>
+      <c r="J20" s="68"/>
       <c r="K20" s="66"/>
     </row>
     <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
@@ -2649,11 +2649,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="79" t="s">
+      <c r="J22" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="79"/>
-      <c r="L22" s="79"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
     </row>
     <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -2977,22 +2977,22 @@
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B41" s="59" t="s">
+      <c r="B41" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="60"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="61"/>
     </row>
     <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="61"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="62"/>
+      <c r="B42" s="64"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="65"/>
+      <c r="G42" s="65"/>
     </row>
     <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
@@ -3664,14 +3664,14 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="59" t="s">
+      <c r="B72" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="60"/>
-      <c r="D72" s="60"/>
-      <c r="E72" s="60"/>
-      <c r="F72" s="60"/>
-      <c r="G72" s="60"/>
+      <c r="C72" s="61"/>
+      <c r="D72" s="61"/>
+      <c r="E72" s="61"/>
+      <c r="F72" s="61"/>
+      <c r="G72" s="61"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3683,12 +3683,12 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="61"/>
-      <c r="C73" s="62"/>
-      <c r="D73" s="62"/>
-      <c r="E73" s="62"/>
-      <c r="F73" s="62"/>
-      <c r="G73" s="62"/>
+      <c r="B73" s="64"/>
+      <c r="C73" s="65"/>
+      <c r="D73" s="65"/>
+      <c r="E73" s="65"/>
+      <c r="F73" s="65"/>
+      <c r="G73" s="65"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -4648,22 +4648,22 @@
       <c r="G126" s="50"/>
     </row>
     <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="59" t="s">
+      <c r="B127" s="60" t="s">
         <v>176</v>
       </c>
-      <c r="C127" s="60"/>
-      <c r="D127" s="60"/>
-      <c r="E127" s="60"/>
-      <c r="F127" s="60"/>
-      <c r="G127" s="60"/>
+      <c r="C127" s="61"/>
+      <c r="D127" s="61"/>
+      <c r="E127" s="61"/>
+      <c r="F127" s="61"/>
+      <c r="G127" s="61"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="80"/>
-      <c r="C128" s="81"/>
-      <c r="D128" s="81"/>
-      <c r="E128" s="81"/>
-      <c r="F128" s="81"/>
-      <c r="G128" s="81"/>
+      <c r="B128" s="62"/>
+      <c r="C128" s="63"/>
+      <c r="D128" s="63"/>
+      <c r="E128" s="63"/>
+      <c r="F128" s="63"/>
+      <c r="G128" s="63"/>
     </row>
     <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="51" t="s">
@@ -4803,7 +4803,9 @@
       <c r="C134" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="D134" s="13"/>
+      <c r="D134" s="15">
+        <v>29</v>
+      </c>
       <c r="E134" s="13">
         <v>6</v>
       </c>
@@ -4949,22 +4951,22 @@
       <c r="G141" s="7"/>
     </row>
     <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="59" t="s">
+      <c r="B142" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="C142" s="60"/>
-      <c r="D142" s="60"/>
-      <c r="E142" s="60"/>
-      <c r="F142" s="60"/>
-      <c r="G142" s="60"/>
+      <c r="C142" s="61"/>
+      <c r="D142" s="61"/>
+      <c r="E142" s="61"/>
+      <c r="F142" s="61"/>
+      <c r="G142" s="61"/>
     </row>
     <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="80"/>
-      <c r="C143" s="81"/>
-      <c r="D143" s="81"/>
-      <c r="E143" s="81"/>
-      <c r="F143" s="81"/>
-      <c r="G143" s="81"/>
+      <c r="B143" s="62"/>
+      <c r="C143" s="63"/>
+      <c r="D143" s="63"/>
+      <c r="E143" s="63"/>
+      <c r="F143" s="63"/>
+      <c r="G143" s="63"/>
     </row>
     <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="55" t="s">
@@ -4973,14 +4975,16 @@
       <c r="C144" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="D144" s="13"/>
+      <c r="D144" s="15">
+        <v>29</v>
+      </c>
       <c r="E144" s="13">
         <v>1</v>
       </c>
       <c r="F144" s="13">
         <v>3</v>
       </c>
-      <c r="G144" s="13"/>
+      <c r="G144" s="7"/>
       <c r="I144" s="58" t="s">
         <v>188</v>
       </c>
@@ -4998,10 +5002,16 @@
       <c r="C145" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="D145" s="13"/>
-      <c r="E145" s="13"/>
-      <c r="F145" s="13"/>
-      <c r="G145" s="13"/>
+      <c r="D145" s="15">
+        <v>45</v>
+      </c>
+      <c r="E145" s="13">
+        <v>2</v>
+      </c>
+      <c r="F145" s="13">
+        <v>7</v>
+      </c>
+      <c r="G145" s="11"/>
       <c r="I145" s="57" t="s">
         <v>9</v>
       </c>
@@ -5071,12 +5081,12 @@
         <v>12</v>
       </c>
       <c r="J148">
-        <f>F144</f>
+        <f>F144+F145+F147</f>
+        <v>10</v>
+      </c>
+      <c r="K148">
+        <f>E144+E145+E147</f>
         <v>3</v>
-      </c>
-      <c r="K148">
-        <f>E144</f>
-        <v>1</v>
       </c>
     </row>
     <row r="149" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5213,11 +5223,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="B142:G143"/>
-    <mergeCell ref="B127:G128"/>
-    <mergeCell ref="B72:G73"/>
-    <mergeCell ref="B41:G42"/>
+    <mergeCell ref="B4:G5"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="K15:K17"/>
     <mergeCell ref="K18:K20"/>
     <mergeCell ref="J18:J20"/>
     <mergeCell ref="K3:K5"/>
@@ -5225,11 +5235,11 @@
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
-    <mergeCell ref="B4:G5"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="B142:G143"/>
+    <mergeCell ref="B127:G128"/>
+    <mergeCell ref="B72:G73"/>
+    <mergeCell ref="B41:G42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5245,8 +5255,8 @@
   </sheetPr>
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5286,7 +5296,7 @@
       </c>
       <c r="K1" s="2">
         <f>SUM(B2:B1000)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5810,7 +5820,9 @@
       <c r="A30" s="15">
         <v>29</v>
       </c>
-      <c r="B30" s="18"/>
+      <c r="B30" s="17">
+        <v>1</v>
+      </c>
       <c r="C30" s="16" t="s">
         <v>128</v>
       </c>
@@ -6134,7 +6146,9 @@
       <c r="A46" s="15">
         <v>45</v>
       </c>
-      <c r="B46" s="18"/>
+      <c r="B46" s="17">
+        <v>1</v>
+      </c>
       <c r="C46" s="16" t="s">
         <v>142</v>
       </c>
@@ -6215,6 +6229,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6423,38 +6454,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6477,9 +6480,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Titulos web de ruleta rusa, soporte cliente y desafios y recompensas
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 5ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 5ª Version.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF9CFFE-BC0E-4F4C-AD5D-0571A92D43A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDD883B-2C36-4AB1-A23B-063A458C4EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -1119,19 +1119,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1140,7 +1131,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1170,23 +1179,14 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2208,7 +2208,7 @@
   </sheetPr>
   <dimension ref="A2:P156"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B142" sqref="B142:G143"/>
     </sheetView>
   </sheetViews>
@@ -2267,34 +2267,34 @@
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="69">
+      <c r="K3" s="72">
         <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130</f>
         <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="69"/>
+      <c r="K4" s="72"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="64"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="69"/>
+      <c r="K5" s="72"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2314,7 +2314,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="70" t="s">
+      <c r="J6" s="73" t="s">
         <v>12</v>
       </c>
       <c r="K6" s="66">
@@ -2340,7 +2340,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="71"/>
+      <c r="J7" s="74"/>
       <c r="K7" s="66"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -2361,7 +2361,7 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="72"/>
+      <c r="J8" s="75"/>
       <c r="K8" s="66"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -2382,7 +2382,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="73" t="s">
+      <c r="J9" s="76" t="s">
         <v>13</v>
       </c>
       <c r="K9" s="66">
@@ -2407,7 +2407,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="74"/>
+      <c r="J10" s="77"/>
       <c r="K10" s="66"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2425,7 +2425,7 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="75"/>
+      <c r="J11" s="78"/>
       <c r="K11" s="66"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -2445,7 +2445,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="76" t="s">
+      <c r="J12" s="63" t="s">
         <v>14</v>
       </c>
       <c r="K12" s="66">
@@ -2468,7 +2468,7 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="77"/>
+      <c r="J13" s="64"/>
       <c r="K13" s="66"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2486,7 +2486,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="78"/>
+      <c r="J14" s="65"/>
       <c r="K14" s="66"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2504,7 +2504,7 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="79" t="s">
+      <c r="J15" s="67" t="s">
         <v>15</v>
       </c>
       <c r="K15" s="66">
@@ -2527,7 +2527,7 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="80"/>
+      <c r="J16" s="68"/>
       <c r="K16" s="66"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2545,7 +2545,7 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="81"/>
+      <c r="J17" s="69"/>
       <c r="K17" s="66"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2565,7 +2565,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="67" t="s">
+      <c r="J18" s="70" t="s">
         <v>16</v>
       </c>
       <c r="K18" s="66">
@@ -2591,7 +2591,7 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="68"/>
+      <c r="J19" s="71"/>
       <c r="K19" s="66"/>
     </row>
     <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
@@ -2611,7 +2611,7 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="68"/>
+      <c r="J20" s="71"/>
       <c r="K20" s="66"/>
     </row>
     <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
@@ -2649,11 +2649,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="59" t="s">
+      <c r="J22" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="59"/>
-      <c r="L22" s="59"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="79"/>
     </row>
     <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -2977,22 +2977,22 @@
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B41" s="60" t="s">
+      <c r="B41" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
     </row>
     <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B42" s="64"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
     </row>
     <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
@@ -3664,14 +3664,14 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="60" t="s">
+      <c r="B72" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="61"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="61"/>
-      <c r="G72" s="61"/>
+      <c r="C72" s="60"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="60"/>
+      <c r="F72" s="60"/>
+      <c r="G72" s="60"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3683,12 +3683,12 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="64"/>
-      <c r="C73" s="65"/>
-      <c r="D73" s="65"/>
-      <c r="E73" s="65"/>
-      <c r="F73" s="65"/>
-      <c r="G73" s="65"/>
+      <c r="B73" s="61"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="62"/>
+      <c r="E73" s="62"/>
+      <c r="F73" s="62"/>
+      <c r="G73" s="62"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -4648,22 +4648,22 @@
       <c r="G126" s="50"/>
     </row>
     <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="60" t="s">
+      <c r="B127" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="C127" s="61"/>
-      <c r="D127" s="61"/>
-      <c r="E127" s="61"/>
-      <c r="F127" s="61"/>
-      <c r="G127" s="61"/>
+      <c r="C127" s="60"/>
+      <c r="D127" s="60"/>
+      <c r="E127" s="60"/>
+      <c r="F127" s="60"/>
+      <c r="G127" s="60"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="62"/>
-      <c r="C128" s="63"/>
-      <c r="D128" s="63"/>
-      <c r="E128" s="63"/>
-      <c r="F128" s="63"/>
-      <c r="G128" s="63"/>
+      <c r="B128" s="80"/>
+      <c r="C128" s="81"/>
+      <c r="D128" s="81"/>
+      <c r="E128" s="81"/>
+      <c r="F128" s="81"/>
+      <c r="G128" s="81"/>
     </row>
     <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="51" t="s">
@@ -4951,22 +4951,22 @@
       <c r="G141" s="7"/>
     </row>
     <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="60" t="s">
+      <c r="B142" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="C142" s="61"/>
-      <c r="D142" s="61"/>
-      <c r="E142" s="61"/>
-      <c r="F142" s="61"/>
-      <c r="G142" s="61"/>
+      <c r="C142" s="60"/>
+      <c r="D142" s="60"/>
+      <c r="E142" s="60"/>
+      <c r="F142" s="60"/>
+      <c r="G142" s="60"/>
     </row>
     <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="62"/>
-      <c r="C143" s="63"/>
-      <c r="D143" s="63"/>
-      <c r="E143" s="63"/>
-      <c r="F143" s="63"/>
-      <c r="G143" s="63"/>
+      <c r="B143" s="80"/>
+      <c r="C143" s="81"/>
+      <c r="D143" s="81"/>
+      <c r="E143" s="81"/>
+      <c r="F143" s="81"/>
+      <c r="G143" s="81"/>
     </row>
     <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="55" t="s">
@@ -5223,11 +5223,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B4:G5"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="B142:G143"/>
+    <mergeCell ref="B127:G128"/>
+    <mergeCell ref="B72:G73"/>
+    <mergeCell ref="B41:G42"/>
     <mergeCell ref="K18:K20"/>
     <mergeCell ref="J18:J20"/>
     <mergeCell ref="K3:K5"/>
@@ -5235,11 +5235,11 @@
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="B142:G143"/>
-    <mergeCell ref="B127:G128"/>
-    <mergeCell ref="B72:G73"/>
-    <mergeCell ref="B41:G42"/>
+    <mergeCell ref="B4:G5"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="K15:K17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5255,7 +5255,7 @@
   </sheetPr>
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -6229,23 +6229,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6454,10 +6437,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6480,20 +6491,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
El excel va peor que la ruleta
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 5ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 5ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahdm\Workspace\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanzc\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4EB3F2-33DA-4FF7-A40A-3F464444A0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0848881B-EE72-42AD-9AEA-234AEFE0C83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="201">
   <si>
     <t>Nombre</t>
   </si>
@@ -666,6 +666,9 @@
   </si>
   <si>
     <t>Lógica 1 jugador Póker Texas</t>
+  </si>
+  <si>
+    <t>Ayuda perfil toolbar</t>
   </si>
 </sst>
 </file>
@@ -1119,19 +1122,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1140,7 +1134,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1170,23 +1182,14 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2206,10 +2209,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:P156"/>
+  <dimension ref="A2:P158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F153" sqref="F153"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2259,42 +2262,42 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E996)</f>
-        <v>330.2</v>
+        <v>341.2</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>437.03000000000003</v>
+        <v>453.03000000000003</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="69">
-        <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130</f>
-        <v>103</v>
+      <c r="K3" s="72">
+        <f>F6+F12+F22+F21+F52+F53+F54+F62+F63+F64+F65+F71+J73+J130+J145</f>
+        <v>121.5</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
       <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="69"/>
+      <c r="K4" s="72"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="64"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="69"/>
+      <c r="K5" s="72"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -2314,7 +2317,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="70" t="s">
+      <c r="J6" s="73" t="s">
         <v>12</v>
       </c>
       <c r="K6" s="66">
@@ -2340,7 +2343,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="71"/>
+      <c r="J7" s="74"/>
       <c r="K7" s="66"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -2361,7 +2364,7 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="72"/>
+      <c r="J8" s="75"/>
       <c r="K8" s="66"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -2382,7 +2385,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="73" t="s">
+      <c r="J9" s="76" t="s">
         <v>13</v>
       </c>
       <c r="K9" s="66">
@@ -2407,7 +2410,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="74"/>
+      <c r="J10" s="77"/>
       <c r="K10" s="66"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2425,7 +2428,7 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="75"/>
+      <c r="J11" s="78"/>
       <c r="K11" s="66"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -2445,12 +2448,12 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="76" t="s">
+      <c r="J12" s="63" t="s">
         <v>14</v>
       </c>
       <c r="K12" s="66">
-        <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77+J134</f>
-        <v>62.85</v>
+        <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F48+F67+F68+J77+J134+J149</f>
+        <v>78.849999999999994</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2468,7 +2471,7 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="77"/>
+      <c r="J13" s="64"/>
       <c r="K13" s="66"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2486,7 +2489,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="78"/>
+      <c r="J14" s="65"/>
       <c r="K14" s="66"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2504,7 +2507,7 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="79" t="s">
+      <c r="J15" s="67" t="s">
         <v>15</v>
       </c>
       <c r="K15" s="66">
@@ -2527,7 +2530,7 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="80"/>
+      <c r="J16" s="68"/>
       <c r="K16" s="66"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2545,7 +2548,7 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="81"/>
+      <c r="J17" s="69"/>
       <c r="K17" s="66"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2565,7 +2568,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="67" t="s">
+      <c r="J18" s="70" t="s">
         <v>16</v>
       </c>
       <c r="K18" s="66">
@@ -2591,7 +2594,7 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="68"/>
+      <c r="J19" s="71"/>
       <c r="K19" s="66"/>
     </row>
     <row r="20" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
@@ -2611,7 +2614,7 @@
         <v>20</v>
       </c>
       <c r="G20" s="41"/>
-      <c r="J20" s="68"/>
+      <c r="J20" s="71"/>
       <c r="K20" s="66"/>
     </row>
     <row r="21" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
@@ -2649,11 +2652,11 @@
         <v>5</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="J22" s="59" t="s">
+      <c r="J22" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="59"/>
-      <c r="L22" s="59"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="79"/>
     </row>
     <row r="23" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -2977,22 +2980,22 @@
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B41" s="60" t="s">
+      <c r="B41" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
     </row>
     <row r="42" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B42" s="64"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
     </row>
     <row r="43" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
@@ -3664,14 +3667,14 @@
       <c r="G71" s="7"/>
     </row>
     <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="60" t="s">
+      <c r="B72" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="61"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="61"/>
-      <c r="G72" s="61"/>
+      <c r="C72" s="60"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="60"/>
+      <c r="F72" s="60"/>
+      <c r="G72" s="60"/>
       <c r="I72" s="33" t="s">
         <v>68</v>
       </c>
@@ -3683,12 +3686,12 @@
       </c>
     </row>
     <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="64"/>
-      <c r="C73" s="65"/>
-      <c r="D73" s="65"/>
-      <c r="E73" s="65"/>
-      <c r="F73" s="65"/>
-      <c r="G73" s="65"/>
+      <c r="B73" s="61"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="62"/>
+      <c r="E73" s="62"/>
+      <c r="F73" s="62"/>
+      <c r="G73" s="62"/>
       <c r="I73" s="4" t="s">
         <v>9</v>
       </c>
@@ -4648,22 +4651,22 @@
       <c r="G126" s="50"/>
     </row>
     <row r="127" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="60" t="s">
+      <c r="B127" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="C127" s="61"/>
-      <c r="D127" s="61"/>
-      <c r="E127" s="61"/>
-      <c r="F127" s="61"/>
-      <c r="G127" s="61"/>
+      <c r="C127" s="60"/>
+      <c r="D127" s="60"/>
+      <c r="E127" s="60"/>
+      <c r="F127" s="60"/>
+      <c r="G127" s="60"/>
     </row>
     <row r="128" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="62"/>
-      <c r="C128" s="63"/>
-      <c r="D128" s="63"/>
-      <c r="E128" s="63"/>
-      <c r="F128" s="63"/>
-      <c r="G128" s="63"/>
+      <c r="B128" s="80"/>
+      <c r="C128" s="81"/>
+      <c r="D128" s="81"/>
+      <c r="E128" s="81"/>
+      <c r="F128" s="81"/>
+      <c r="G128" s="81"/>
     </row>
     <row r="129" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="51" t="s">
@@ -4951,22 +4954,22 @@
       <c r="G141" s="7"/>
     </row>
     <row r="142" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="60" t="s">
+      <c r="B142" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="C142" s="61"/>
-      <c r="D142" s="61"/>
-      <c r="E142" s="61"/>
-      <c r="F142" s="61"/>
-      <c r="G142" s="61"/>
+      <c r="C142" s="60"/>
+      <c r="D142" s="60"/>
+      <c r="E142" s="60"/>
+      <c r="F142" s="60"/>
+      <c r="G142" s="60"/>
     </row>
     <row r="143" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="62"/>
-      <c r="C143" s="63"/>
-      <c r="D143" s="63"/>
-      <c r="E143" s="63"/>
-      <c r="F143" s="63"/>
-      <c r="G143" s="63"/>
+      <c r="B143" s="80"/>
+      <c r="C143" s="81"/>
+      <c r="D143" s="81"/>
+      <c r="E143" s="81"/>
+      <c r="F143" s="81"/>
+      <c r="G143" s="81"/>
     </row>
     <row r="144" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="55" t="s">
@@ -5109,6 +5112,10 @@
       <c r="I149" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="J149">
+        <f>F157+F158</f>
+        <v>16</v>
+      </c>
     </row>
     <row r="150" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="52" t="s">
@@ -5223,13 +5230,45 @@
       <c r="F156" s="13"/>
       <c r="G156" s="11"/>
     </row>
+    <row r="157" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B157" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C157" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D157" s="13"/>
+      <c r="E157" s="13">
+        <v>10</v>
+      </c>
+      <c r="F157" s="13">
+        <v>15</v>
+      </c>
+      <c r="G157" s="11"/>
+    </row>
+    <row r="158" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B158" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C158" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="D158" s="13"/>
+      <c r="E158" s="13">
+        <v>1</v>
+      </c>
+      <c r="F158" s="13">
+        <v>1</v>
+      </c>
+      <c r="G158" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B4:G5"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="B142:G143"/>
+    <mergeCell ref="B127:G128"/>
+    <mergeCell ref="B72:G73"/>
+    <mergeCell ref="B41:G42"/>
     <mergeCell ref="K18:K20"/>
     <mergeCell ref="J18:J20"/>
     <mergeCell ref="K3:K5"/>
@@ -5237,11 +5276,11 @@
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="B142:G143"/>
-    <mergeCell ref="B127:G128"/>
-    <mergeCell ref="B72:G73"/>
-    <mergeCell ref="B41:G42"/>
+    <mergeCell ref="B4:G5"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="K15:K17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6231,23 +6270,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -6456,10 +6478,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6482,20 +6532,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>